<commit_message>
Fix issue seeding jurisdiction HDD
[BPHH-2630]
</commit_message>
<xml_diff>
--- a/db/templates/jurisdiction_hdd_references.xlsx
+++ b/db/templates/jurisdiction_hdd_references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurelolson/dev_work/HOUS-permit-portal/db/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0534D63-BC45-CF42-9ABF-82BF23894155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C66A8C-12DE-7242-9DD4-9C7E08D93A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{92118432-263E-6A4D-832F-45EE8D3E5F00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="426">
   <si>
     <t>AHJs</t>
   </si>
@@ -944,571 +944,376 @@
     <t>Youbou</t>
   </si>
   <si>
-    <t>5be29c6d-7d6e-4966-9d9f-94aa9c948464</t>
-  </si>
-  <si>
-    <t>d9c367b4-531b-41a9-941a-fa5d04b7d5d2</t>
-  </si>
-  <si>
-    <t>f2b5c95e-7190-477e-97cd-7a67bb3085c8</t>
-  </si>
-  <si>
-    <t>54aa7568-ab3e-42d8-bf86-60bee1355794</t>
-  </si>
-  <si>
-    <t>c0e8702c-c397-4f2a-864c-768e2edc5338</t>
-  </si>
-  <si>
-    <t>c8d0c450-5c28-4c5a-aa06-91506f6f747a</t>
-  </si>
-  <si>
-    <t>004a185e-5631-4a1f-ae4c-545a84d6530c</t>
-  </si>
-  <si>
-    <t>c0f3a3df-6ed3-4eb0-b305-a90c8a851d69</t>
-  </si>
-  <si>
-    <t>b1556ed7-5fc3-4f2c-bff2-16acdfa86788</t>
-  </si>
-  <si>
-    <t>35d987c7-e116-4726-a5a0-3a9b16bd6656</t>
-  </si>
-  <si>
-    <t>e73870c1-de94-45b0-9bbf-f00917846f3a</t>
-  </si>
-  <si>
-    <t>afe39199-abfe-4546-84ee-cfa5f3625ba9</t>
-  </si>
-  <si>
-    <t>e71d21f1-731b-4123-9f05-eafd4bd1fcd8</t>
-  </si>
-  <si>
-    <t>a8e008e4-e98b-4fff-94f3-946c04d79f21</t>
-  </si>
-  <si>
-    <t>f519cf18-639c-42f6-a38a-a8d58c73a221</t>
-  </si>
-  <si>
-    <t>5ce75caf-afb2-4f30-9189-6215e2a28721</t>
-  </si>
-  <si>
-    <t>c7ef2b8a-1d8b-4475-8b1a-c8e5ece85e1a</t>
-  </si>
-  <si>
-    <t>50f9559d-a391-4064-966b-474b146cea84</t>
-  </si>
-  <si>
-    <t>73f80e9e-bc85-4a03-9acc-3971f6fd3077</t>
-  </si>
-  <si>
-    <t>5f266b2c-7e60-4f78-8852-87942533fda2</t>
-  </si>
-  <si>
-    <t>8bec8283-2bdd-4abb-b5c0-e746ce43bc27</t>
-  </si>
-  <si>
-    <t>c2177642-b322-458a-b758-b2d03fc13618</t>
-  </si>
-  <si>
-    <t>2653d529-3b16-40bd-832a-d5d79de6add6</t>
-  </si>
-  <si>
-    <t>f0f53f7e-9ef7-477d-b747-4a230e578b24</t>
-  </si>
-  <si>
-    <t>447d6f13-cfd6-4d28-8eee-67e5c619eb16</t>
-  </si>
-  <si>
-    <t>aed389a2-f748-44ce-b71a-ce7bfb8d298c</t>
-  </si>
-  <si>
-    <t>c10b510f-3a73-4a63-96a0-653fe159d860</t>
-  </si>
-  <si>
-    <t>a45ffa41-0984-4745-8e15-a5fc0e55c1d5</t>
-  </si>
-  <si>
-    <t>c16e9b39-f8dd-4f0e-843e-7e20dadcd1da</t>
-  </si>
-  <si>
-    <t>e5bdcc61-79d1-4ebd-835b-4185213c6564</t>
-  </si>
-  <si>
-    <t>f0bbc92e-2536-4257-9075-6b59a01c7f5f</t>
-  </si>
-  <si>
-    <t>fa27871d-21c4-44a2-857c-2e4fc74a4b9f</t>
-  </si>
-  <si>
-    <t>44bb0466-75ad-45b9-932d-39ad4e065929</t>
-  </si>
-  <si>
-    <t>cd73c7a6-5bcd-4aec-97e7-371c2e51e71b</t>
-  </si>
-  <si>
-    <t>91f29223-97e4-4a49-8ff4-f831faeae676</t>
-  </si>
-  <si>
-    <t>aa8a0410-dd6c-4062-95e9-230c06bacaf8</t>
-  </si>
-  <si>
-    <t>7090864e-74a3-4165-888a-5fd27e6f913f</t>
-  </si>
-  <si>
-    <t>10937a22-23fc-47da-970c-a7100c901ec1</t>
-  </si>
-  <si>
-    <t>def4bb78-09a0-48ef-b616-f613476584e6</t>
-  </si>
-  <si>
-    <t>b87f6513-208f-4670-a04e-ec37e8e86f8e</t>
-  </si>
-  <si>
-    <t>c8df55e3-0499-4911-8090-34b62033d630</t>
-  </si>
-  <si>
-    <t>e4872f98-beea-4c86-95ff-d1925bfc1846</t>
-  </si>
-  <si>
-    <t>eb6884fc-49e5-4274-9b07-585ddd862dcd</t>
-  </si>
-  <si>
-    <t>2b7ae013-5abe-49b4-9b16-17876b44d94a</t>
-  </si>
-  <si>
-    <t>78bb21a4-bba4-4f68-8146-5a3a7aed3e7c</t>
-  </si>
-  <si>
-    <t>b5682fe2-b54a-4437-b82a-7da35be6d70f</t>
-  </si>
-  <si>
-    <t>c51b3c04-284a-40f7-a10e-fea2a46f042a</t>
-  </si>
-  <si>
-    <t>9db61d38-973f-45ab-b9fc-0b366c654669</t>
-  </si>
-  <si>
-    <t>a1d40a0d-35ca-48e6-91d5-5bdf47996752</t>
-  </si>
-  <si>
-    <t>e63bcb7c-ee3e-481b-92c2-b48cbb65cf9c</t>
-  </si>
-  <si>
-    <t>946e1f63-61a6-4fcd-9ea5-bfa73d13f4ce</t>
-  </si>
-  <si>
-    <t>44dccc62-d7e2-4fab-a7bd-d7d8c9e50791</t>
-  </si>
-  <si>
-    <t>21790047-236c-4866-bef6-81f27808a6f5</t>
-  </si>
-  <si>
-    <t>5fe550f6-481c-4f32-8ec8-09089f93941c</t>
-  </si>
-  <si>
-    <t>04917f07-cd7a-46c0-87c7-492e4caeb91e</t>
-  </si>
-  <si>
-    <t>3bb93871-39c4-4f47-8516-0a43625663cd</t>
-  </si>
-  <si>
-    <t>4779f2cf-f96b-4e8e-a2a8-febc332fb278</t>
-  </si>
-  <si>
-    <t>4a3b0cef-28bf-4c27-bf7a-4973f6586a11</t>
-  </si>
-  <si>
-    <t>c7e66a46-47b7-4a82-b677-386fc26d322a</t>
-  </si>
-  <si>
-    <t>0f3e49f1-0b33-4623-9813-9db4417ab631</t>
-  </si>
-  <si>
-    <t>6ba1b8d5-a2dc-4229-935e-f7ac54db919c</t>
-  </si>
-  <si>
-    <t>8d36d5ad-4ff8-4d85-b42c-64b08ae2e950</t>
-  </si>
-  <si>
-    <t>06cdce5a-362d-4d7b-9af3-b30721594e6f</t>
-  </si>
-  <si>
-    <t>7a3ea479-e4f3-4910-8eee-2d2df3642642</t>
-  </si>
-  <si>
-    <t>8f32c002-d829-441c-b0d5-25242279a70b</t>
-  </si>
-  <si>
-    <t>940377ce-8147-4cd0-bd27-dbd3ee3a8d2d</t>
-  </si>
-  <si>
-    <t>6f2fdde4-2516-4ae1-9452-dd7b6c191f6a</t>
-  </si>
-  <si>
-    <t>c4e6ee31-28a7-47a2-9aef-d24cbf88c387</t>
-  </si>
-  <si>
-    <t>7d42d620-0a18-4d58-bb6b-d44bc59e4029</t>
-  </si>
-  <si>
-    <t>7bcd04fa-4fc5-4cbf-98f9-0f880d9fa1a2</t>
-  </si>
-  <si>
-    <t>d7a69852-7de6-4176-81aa-0daac89b9365</t>
-  </si>
-  <si>
-    <t>cb58e6e2-636b-416e-9134-c888e6d78ac8</t>
-  </si>
-  <si>
-    <t>c4591ba6-bdd4-42ef-aecc-560b249a4c32</t>
-  </si>
-  <si>
-    <t>cb73240d-d18f-4e56-8379-dd27dabc84fd</t>
-  </si>
-  <si>
-    <t>b9441b1e-af94-44e3-ba01-255909badcb3</t>
-  </si>
-  <si>
-    <t>da7e2937-4c93-4876-a948-adac23218894</t>
-  </si>
-  <si>
-    <t>c9cea64e-84ec-45e0-9810-b68c7fb2f22d</t>
-  </si>
-  <si>
-    <t>1c45169a-16c5-4d32-be21-a9cda5fcb612</t>
-  </si>
-  <si>
-    <t>057909e2-13ec-4d36-8141-f247b86d2ef9</t>
-  </si>
-  <si>
-    <t>b6b29dd5-af35-4181-9503-4f19a5522acd</t>
-  </si>
-  <si>
-    <t>599c709c-b9c2-495e-8738-71b66e5ebbc0</t>
-  </si>
-  <si>
-    <t>a53bffb0-32eb-4216-8b5d-38ba8fe73043</t>
-  </si>
-  <si>
-    <t>fea8996d-9ed5-4aa1-9d1e-8a67948501d2</t>
-  </si>
-  <si>
-    <t>27bb3fae-4b3b-4479-bd8a-ea81005def7e</t>
-  </si>
-  <si>
-    <t>6e696060-ccba-4812-9730-e0206e06757a</t>
-  </si>
-  <si>
-    <t>a474b043-cbb2-492d-9bef-0664bd466be0</t>
-  </si>
-  <si>
-    <t>82fd2e4d-e0fe-4ebc-b7da-ee8ee2f68db6</t>
-  </si>
-  <si>
-    <t>2caefcf6-24d5-4074-aef0-7479b8b10530</t>
-  </si>
-  <si>
-    <t>a15c0cdf-94a8-42fc-9831-d6a8ea180abd</t>
-  </si>
-  <si>
-    <t>0a93c3c2-e3df-46d3-8f41-71f7f406cb0e</t>
-  </si>
-  <si>
-    <t>4b1e10d4-460f-47ad-bc5c-261e56fc02d5</t>
-  </si>
-  <si>
-    <t>492f1daa-3d11-42b1-b95f-087d2e3adda3</t>
-  </si>
-  <si>
-    <t>192e332b-4112-412e-b3e4-25d3d830609a</t>
-  </si>
-  <si>
-    <t>d94df60c-533c-4a96-91e7-23c3f7c033e4</t>
-  </si>
-  <si>
-    <t>3fb25f8a-4a4d-42c2-a6c5-4b8d7686837c</t>
-  </si>
-  <si>
-    <t>080f8d53-9876-4edb-89d0-8a3f4d7c0e92</t>
-  </si>
-  <si>
-    <t>715f5aba-f7fc-4acf-a6f6-65eb913e9caa</t>
-  </si>
-  <si>
-    <t>6dd170e1-5780-4901-b0bc-9f5d4462bfd0</t>
-  </si>
-  <si>
-    <t>2724d97f-80ee-474a-b1f8-c5969a143e3b</t>
-  </si>
-  <si>
-    <t>5edba789-1e39-4edf-aac9-ea0978e82a5b</t>
-  </si>
-  <si>
-    <t>45584a65-61c8-4bff-a3dd-36170fe2f26b</t>
-  </si>
-  <si>
-    <t>bd7ee503-9b06-4a0b-8384-a6c02ad92382</t>
-  </si>
-  <si>
-    <t>13104e6d-8500-48a3-8422-bfaeaf8a5d73</t>
-  </si>
-  <si>
-    <t>715e0910-775f-4913-81f4-ff0f1838d8b3</t>
-  </si>
-  <si>
-    <t>b0c4ba51-749f-41cd-b1e4-6117206fc111</t>
-  </si>
-  <si>
-    <t>c98ff0a4-aa47-481e-9e98-534d7ddf57d4</t>
-  </si>
-  <si>
-    <t>f8368dc4-e3cc-4656-867d-dee7407d0249</t>
-  </si>
-  <si>
-    <t>ce41ba5a-2ad0-4e93-9472-70c896f59fc3</t>
-  </si>
-  <si>
-    <t>a739552e-7245-457a-8ec1-7de32e4ce26a</t>
-  </si>
-  <si>
-    <t>01be55cb-4568-4c70-960e-4490a68dadc8</t>
-  </si>
-  <si>
-    <t>183f7c5b-04e4-40d1-8aec-68c32b84b718</t>
-  </si>
-  <si>
-    <t>2db40b03-6e6b-4d06-b49d-2b21d62127bf</t>
-  </si>
-  <si>
-    <t>c56ca10f-9ffc-4b7b-9083-f37a32ec2be2</t>
-  </si>
-  <si>
-    <t>8531abe3-367a-4977-8aef-cd857c40ede9</t>
-  </si>
-  <si>
-    <t>ed5f82c1-bd71-410d-b06f-c605bb74d3fd</t>
-  </si>
-  <si>
-    <t>8cd2c3da-507c-4eeb-8ffe-d2a72db59a50</t>
-  </si>
-  <si>
-    <t>877206a1-b00d-4d55-b46f-dd845e9dcd3c</t>
-  </si>
-  <si>
-    <t>95e3b7d5-6143-4a98-922b-220ec82655be</t>
-  </si>
-  <si>
-    <t>eb7259cd-7011-497e-affc-61cc8c396e52</t>
-  </si>
-  <si>
-    <t>59120c4c-2140-4f0c-838d-a9de43e57c5d</t>
-  </si>
-  <si>
-    <t>d4766d60-289b-4bf0-b7eb-bef9429fa926</t>
-  </si>
-  <si>
-    <t>c76016be-e4a3-464d-a379-686d026e4b6d</t>
-  </si>
-  <si>
-    <t>c12072e4-f30b-43c4-9678-8299ab5fb665</t>
-  </si>
-  <si>
-    <t>aa3ecc51-9d5a-4147-85f0-813dfd3fa79d</t>
-  </si>
-  <si>
-    <t>99d562fa-55a4-491e-ac93-4b1270332c3a</t>
-  </si>
-  <si>
-    <t>b217955e-1799-49c3-b458-61cf4dd04344</t>
-  </si>
-  <si>
-    <t>06112064-5ab7-438c-9c0b-c67d4192cd57</t>
-  </si>
-  <si>
-    <t>d59a2b94-0821-461c-baea-90b2b41e39a8</t>
-  </si>
-  <si>
-    <t>e3a517dc-972f-498f-975b-61eda0ee6d7d</t>
-  </si>
-  <si>
     <t>Port Hardy (District of Port Hardy)</t>
   </si>
   <si>
-    <t>387d3107-7427-4723-ba9f-749036870ecd</t>
-  </si>
-  <si>
-    <t>cc572233-2cf8-4670-b772-55c6d366d5cf</t>
-  </si>
-  <si>
-    <t>d1521cae-f830-465a-a9c8-46596918de94</t>
-  </si>
-  <si>
-    <t>01b8d678-2f28-425e-84bc-5e30de15a0ed</t>
-  </si>
-  <si>
-    <t>b521cf28-7da4-4648-86b3-e1ea8ff976db</t>
-  </si>
-  <si>
-    <t>7ef1601f-2613-40b5-b0be-7e90adba6773</t>
-  </si>
-  <si>
-    <t>c19fab61-e0ad-414b-8230-1b3d083aa53f</t>
-  </si>
-  <si>
-    <t>d97acffd-5fad-41a1-a680-bd6e2ac8aa06</t>
-  </si>
-  <si>
-    <t>df4f04ca-31d6-4751-bd00-4233b91339ee</t>
-  </si>
-  <si>
-    <t>f9c02a36-d52b-441b-9750-dbdd145a3747</t>
-  </si>
-  <si>
-    <t>4d07e1b6-5bef-4099-ab65-1a98336a0877</t>
-  </si>
-  <si>
-    <t>aea37714-ae83-4b67-9174-f0e008ae5a7c</t>
-  </si>
-  <si>
-    <t>eb349e5f-6d57-4267-ac19-8af9797e2432</t>
-  </si>
-  <si>
-    <t>63f244c1-a1e0-413b-8cf9-84529e2fbb1d</t>
-  </si>
-  <si>
-    <t>c57b37f9-3bb4-4ea4-8edc-85446ef3e66a</t>
-  </si>
-  <si>
-    <t>e702a01b-c19d-4f6e-a3ef-0e9f4b6bc02a</t>
-  </si>
-  <si>
-    <t>3f5f5b62-8ae2-4a3b-ab12-68cf07a24e27</t>
-  </si>
-  <si>
-    <t>3925cb9d-c0f4-40a3-b477-a4a0cfe15558</t>
-  </si>
-  <si>
-    <t>a194e17c-4fc1-4636-8fbd-784c7d701e55</t>
-  </si>
-  <si>
-    <t>fc20b65e-f8a0-4138-ba3b-5a33fa0f600d</t>
-  </si>
-  <si>
-    <t>1bf143b4-8dc1-47ca-988b-6a708d8f1d97</t>
-  </si>
-  <si>
-    <t>c6a8acd9-0eb2-439f-8cea-dc90c66885cb</t>
-  </si>
-  <si>
-    <t>ddc9bc81-3f65-44a5-ae18-2c39bcaf48e2</t>
-  </si>
-  <si>
-    <t>bda93f16-bc84-4f9a-9ecc-37afa52b7625</t>
-  </si>
-  <si>
-    <t>94b7927e-29ba-44e5-9a0d-0cc34e048038</t>
-  </si>
-  <si>
-    <t>d462e18a-2aeb-491e-ad4b-8637985ab51f</t>
-  </si>
-  <si>
-    <t>dcdd0423-cfee-4073-bbe8-b7c77997cbe8</t>
-  </si>
-  <si>
-    <t>7b4afc05-580d-4362-bf54-2233623bdfc7</t>
-  </si>
-  <si>
-    <t>999dfef3-b3a6-46de-b395-05e202a8b61b</t>
-  </si>
-  <si>
-    <t>fccd65ab-2843-4746-bcc1-523a31fcd753</t>
-  </si>
-  <si>
-    <t>9d36246a-1be3-4414-8e08-c04aa262f190</t>
-  </si>
-  <si>
-    <t>c50d63b6-5b3d-443e-ba6e-461a16435153</t>
-  </si>
-  <si>
-    <t>5c61efd4-12a5-4b32-9b37-0aa30438f5f9</t>
-  </si>
-  <si>
-    <t>1d89f91f-71fd-44ff-846a-6e247cd4f271</t>
-  </si>
-  <si>
-    <t>4c56691d-29d3-47fa-92fc-69718d2b7a2f</t>
-  </si>
-  <si>
-    <t>eb64a7f7-9493-42de-b8a7-6894210e50aa</t>
-  </si>
-  <si>
-    <t>dd0264bb-8164-4c61-94e1-a93e5e93ca85</t>
-  </si>
-  <si>
-    <t>5f7f97c7-bc99-4121-8fda-d841145fdef6</t>
-  </si>
-  <si>
-    <t>3d64994d-c0be-4319-a1c0-8000d3e9e98e</t>
-  </si>
-  <si>
-    <t>8ae9bd1e-638c-47ba-9d05-95febffff3f2</t>
-  </si>
-  <si>
-    <t>6bf2294a-1b7f-4255-a08a-97037c8cfc3f</t>
-  </si>
-  <si>
-    <t>5fa0692b-6b37-4adc-8983-d5571b539260</t>
-  </si>
-  <si>
-    <t>00447394-a790-490a-9f6a-deaf233a53e0</t>
-  </si>
-  <si>
-    <t>2531e04a-1f63-4b0f-a73e-9ddf6b3ca673</t>
-  </si>
-  <si>
-    <t>5d97e398-793a-4590-ac08-e9a5e0694bd0</t>
-  </si>
-  <si>
-    <t>956159d8-44ef-4fed-b441-1624a3fee05b</t>
-  </si>
-  <si>
-    <t>64ab674b-2153-4989-a0f8-ac1370674e7d</t>
-  </si>
-  <si>
-    <t>b0e62424-4ed5-42a9-bc0f-32825bd9119e</t>
-  </si>
-  <si>
-    <t>df6e4b86-632c-46d8-abb1-fc489fe90993</t>
-  </si>
-  <si>
-    <t>9aec9271-9da1-47d1-9802-5a0a530fa66e</t>
-  </si>
-  <si>
-    <t>4e925b17-7a7d-4c6b-98f2-8f9adfaf03f1</t>
-  </si>
-  <si>
-    <t>7c0c7798-1767-461d-be7a-4e27433c5f96</t>
-  </si>
-  <si>
-    <t>9c671cdd-5026-4d1a-af60-a75854fb0665</t>
-  </si>
-  <si>
-    <t>f749fb0c-232e-4c94-b38e-0bbd93a151c0</t>
-  </si>
-  <si>
-    <t>248367ab-8def-4f5e-9d77-81f7b8b43911</t>
-  </si>
-  <si>
-    <t>495fb564-6d9f-442e-b9ab-721b4668a637</t>
-  </si>
-  <si>
-    <t>fd9f3c09-728a-4054-b20c-e17b6f9cf268</t>
-  </si>
-  <si>
-    <t>f62c9534-0833-4a71-a9ad-d6232c409e3b</t>
-  </si>
-  <si>
-    <t>jurisdiction_id</t>
+    <t>jurisdiction_name</t>
+  </si>
+  <si>
+    <t>locality_type</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Alert Bay</t>
+  </si>
+  <si>
+    <t>corporation of the village</t>
+  </si>
+  <si>
+    <t>Anmore</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>Armstrong</t>
+  </si>
+  <si>
+    <t>Barriere</t>
+  </si>
+  <si>
+    <t>Belcarra</t>
+  </si>
+  <si>
+    <t>Bowen Island</t>
+  </si>
+  <si>
+    <t>municipality</t>
+  </si>
+  <si>
+    <t>Burnaby</t>
+  </si>
+  <si>
+    <t>Canal Flats</t>
+  </si>
+  <si>
+    <t>Central Saanich</t>
+  </si>
+  <si>
+    <t>corporation of the district</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Clearwater</t>
+  </si>
+  <si>
+    <t>Clinton</t>
+  </si>
+  <si>
+    <t>Coldstream</t>
+  </si>
+  <si>
+    <t>Colwood</t>
+  </si>
+  <si>
+    <t>town</t>
+  </si>
+  <si>
+    <t>Coquitlam</t>
+  </si>
+  <si>
+    <t>corporation of the city</t>
+  </si>
+  <si>
+    <t>Creston</t>
+  </si>
+  <si>
+    <t>Cumberland</t>
+  </si>
+  <si>
+    <t>Daajing Giids</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Elkford</t>
+  </si>
+  <si>
+    <t>Enderby</t>
+  </si>
+  <si>
+    <t>Esquimalt</t>
+  </si>
+  <si>
+    <t>corporation of the township</t>
+  </si>
+  <si>
+    <t>Fraser Lake</t>
+  </si>
+  <si>
+    <t>Fruitvale</t>
+  </si>
+  <si>
+    <t>Gibsons</t>
+  </si>
+  <si>
+    <t>Granisle</t>
+  </si>
+  <si>
+    <t>Harrison Hot Springs</t>
+  </si>
+  <si>
+    <t>Hazelton</t>
+  </si>
+  <si>
+    <t>Highlands</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Hudson's Hope</t>
+  </si>
+  <si>
+    <t>Invermere</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Keremeos</t>
+  </si>
+  <si>
+    <t>Kitimat</t>
+  </si>
+  <si>
+    <t>Lake Country</t>
+  </si>
+  <si>
+    <t>Lake Cowichan</t>
+  </si>
+  <si>
+    <t>Lantzville</t>
+  </si>
+  <si>
+    <t>Lions Bay</t>
+  </si>
+  <si>
+    <t>Lumby</t>
+  </si>
+  <si>
+    <t>Maple Ridge</t>
+  </si>
+  <si>
+    <t>Metchosin</t>
+  </si>
+  <si>
+    <t>Midway</t>
+  </si>
+  <si>
+    <t>Mission</t>
+  </si>
+  <si>
+    <t>New Denver</t>
+  </si>
+  <si>
+    <t>North Cowichan</t>
+  </si>
+  <si>
+    <t>North Saanich</t>
+  </si>
+  <si>
+    <t>Northern Rockies</t>
+  </si>
+  <si>
+    <t>regional municipality</t>
+  </si>
+  <si>
+    <t>Oak Bay</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Peachland</t>
+  </si>
+  <si>
+    <t>Pitt Meadows</t>
+  </si>
+  <si>
+    <t>Port Clements</t>
+  </si>
+  <si>
+    <t>Port Edward</t>
+  </si>
+  <si>
+    <t>Port Moody</t>
+  </si>
+  <si>
+    <t>Radium Hot Springs</t>
+  </si>
+  <si>
+    <t>Rossland</t>
+  </si>
+  <si>
+    <t>Saanich</t>
+  </si>
+  <si>
+    <t>Salmo</t>
+  </si>
+  <si>
+    <t>Sayward</t>
+  </si>
+  <si>
+    <t>Sicamous</t>
+  </si>
+  <si>
+    <t>Silverton</t>
+  </si>
+  <si>
+    <t>Slocan</t>
+  </si>
+  <si>
+    <t>Spallumcheen</t>
+  </si>
+  <si>
+    <t>Sparwood</t>
+  </si>
+  <si>
+    <t>Summerland</t>
+  </si>
+  <si>
+    <t>Sun Peaks Mountain</t>
+  </si>
+  <si>
+    <t>resort municipality</t>
+  </si>
+  <si>
+    <t>Surrey</t>
+  </si>
+  <si>
+    <t>Telkwa</t>
+  </si>
+  <si>
+    <t>Tumbler Ridge</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>Vanderhoof</t>
+  </si>
+  <si>
+    <t>View Royal</t>
+  </si>
+  <si>
+    <t>Warfield</t>
+  </si>
+  <si>
+    <t>Wells</t>
+  </si>
+  <si>
+    <t>West Kelowna</t>
+  </si>
+  <si>
+    <t>Zeballos</t>
+  </si>
+  <si>
+    <t>Bulkley-Nechako</t>
+  </si>
+  <si>
+    <t>regional district</t>
+  </si>
+  <si>
+    <t>Cariboo</t>
+  </si>
+  <si>
+    <t>Fraser-Fort George</t>
+  </si>
+  <si>
+    <t>Kitimat-Stikine</t>
+  </si>
+  <si>
+    <t>Peace River</t>
+  </si>
+  <si>
+    <t>North Coast</t>
+  </si>
+  <si>
+    <t>Central Okanagan</t>
+  </si>
+  <si>
+    <t>Fraser Valley</t>
+  </si>
+  <si>
+    <t>Metro Vancouver</t>
+  </si>
+  <si>
+    <t>Okanagan-Similkameen</t>
+  </si>
+  <si>
+    <t>Squamish-Lillooet</t>
+  </si>
+  <si>
+    <t>Central Kootenay</t>
+  </si>
+  <si>
+    <t>Columbia Shuswap</t>
+  </si>
+  <si>
+    <t>East Kootenay</t>
+  </si>
+  <si>
+    <t>Kootenay Boundary</t>
+  </si>
+  <si>
+    <t>North Okanagan</t>
+  </si>
+  <si>
+    <t>Alberni-Clayoquot</t>
+  </si>
+  <si>
+    <t>The Capital</t>
+  </si>
+  <si>
+    <t>Central Coast</t>
+  </si>
+  <si>
+    <t>Comox Valley</t>
+  </si>
+  <si>
+    <t>Cowichan Valley</t>
+  </si>
+  <si>
+    <t>Mount Waddington</t>
+  </si>
+  <si>
+    <t>qathet</t>
+  </si>
+  <si>
+    <t>Sunshine Coast</t>
+  </si>
+  <si>
+    <t>Strathcona</t>
+  </si>
+  <si>
+    <t>Fort St. James</t>
+  </si>
+  <si>
+    <t>Logan Lake</t>
+  </si>
+  <si>
+    <t>New Hazelton</t>
+  </si>
+  <si>
+    <t>Port Coquitlam</t>
+  </si>
+  <si>
+    <t>Pouce Coupe</t>
+  </si>
+  <si>
+    <t>Valemount</t>
+  </si>
+  <si>
+    <t>Thompson-Nicola</t>
   </si>
 </sst>
 </file>
@@ -1643,7 +1448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1690,7 +1495,6 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2025,10 +1829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96291D7F-454B-F64D-9001-0B6A05DDB28B}">
-  <dimension ref="A1:G189"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="J177" sqref="J177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2040,7 +1844,7 @@
     <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>266</v>
       </c>
@@ -2057,10 +1861,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2078,10 +1885,13 @@
         <v>5030</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2099,10 +1909,13 @@
         <v>2860</v>
       </c>
       <c r="G3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>268</v>
       </c>
@@ -2120,10 +1933,13 @@
         <v/>
       </c>
       <c r="G4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+      <c r="H4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>269</v>
       </c>
@@ -2141,10 +1957,13 @@
         <v/>
       </c>
       <c r="G5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+      <c r="H5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -2162,10 +1981,13 @@
         <v/>
       </c>
       <c r="G6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H6" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>270</v>
       </c>
@@ -2183,10 +2005,13 @@
         <v>3700</v>
       </c>
       <c r="G7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>271</v>
       </c>
@@ -2204,10 +2029,13 @@
         <v/>
       </c>
       <c r="G8" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="H8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>272</v>
       </c>
@@ -2225,10 +2053,13 @@
         <v/>
       </c>
       <c r="G9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+      <c r="H9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>273</v>
       </c>
@@ -2246,10 +2077,13 @@
         <v/>
       </c>
       <c r="G10" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+      <c r="H10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -2267,10 +2101,13 @@
         <v>2735</v>
       </c>
       <c r="G11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+      <c r="H11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>274</v>
       </c>
@@ -2288,10 +2125,13 @@
         <v>5450</v>
       </c>
       <c r="G12" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
@@ -2309,10 +2149,13 @@
         <v>3700</v>
       </c>
       <c r="G13" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -2330,10 +2173,13 @@
         <v>3000</v>
       </c>
       <c r="G14" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>23</v>
       </c>
@@ -2353,8 +2199,11 @@
       <c r="G15" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>275</v>
       </c>
@@ -2372,10 +2221,13 @@
         <v>3580</v>
       </c>
       <c r="G16" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
@@ -2393,10 +2245,13 @@
         <v/>
       </c>
       <c r="G17" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>318</v>
+      </c>
+      <c r="H17" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>30</v>
       </c>
@@ -2414,10 +2269,13 @@
         <v/>
       </c>
       <c r="G18" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+      <c r="H18" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -2435,10 +2293,13 @@
         <v>5500</v>
       </c>
       <c r="G19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>276</v>
       </c>
@@ -2456,10 +2317,13 @@
         <v>2780</v>
       </c>
       <c r="G20" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
@@ -2477,10 +2341,13 @@
         <v/>
       </c>
       <c r="G21" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+      <c r="H21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>41</v>
       </c>
@@ -2498,10 +2365,13 @@
         <v/>
       </c>
       <c r="G22" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+      <c r="H22" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
@@ -2519,10 +2389,13 @@
         <v/>
       </c>
       <c r="G23" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="H23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>277</v>
       </c>
@@ -2540,10 +2413,13 @@
         <v/>
       </c>
       <c r="G24" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+      <c r="H24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>278</v>
       </c>
@@ -2561,10 +2437,13 @@
         <v>3100</v>
       </c>
       <c r="G25" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="H25" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>48</v>
       </c>
@@ -2582,10 +2461,13 @@
         <v/>
       </c>
       <c r="G26" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+      <c r="H26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>279</v>
       </c>
@@ -2603,10 +2485,13 @@
         <v>3100</v>
       </c>
       <c r="G27" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>280</v>
       </c>
@@ -2624,10 +2509,13 @@
         <v>4400</v>
       </c>
       <c r="G28" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="H28" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>51</v>
       </c>
@@ -2645,10 +2533,13 @@
         <v/>
       </c>
       <c r="G29" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+      <c r="H29" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>281</v>
       </c>
@@ -2666,10 +2557,13 @@
         <v/>
       </c>
       <c r="G30" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+      <c r="H30" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>56</v>
       </c>
@@ -2687,10 +2581,13 @@
         <v/>
       </c>
       <c r="G31" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="H31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>282</v>
       </c>
@@ -2708,10 +2605,13 @@
         <v>5900</v>
       </c>
       <c r="G32" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="H32" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -2729,10 +2629,13 @@
         <v/>
       </c>
       <c r="G33" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+      <c r="H33" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>283</v>
       </c>
@@ -2750,10 +2653,13 @@
         <v>2980</v>
       </c>
       <c r="G34" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="H34" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
@@ -2771,10 +2677,13 @@
         <v/>
       </c>
       <c r="G35" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+      <c r="H35" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>66</v>
       </c>
@@ -2792,10 +2701,13 @@
         <v/>
       </c>
       <c r="G36" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+      <c r="H36" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>68</v>
       </c>
@@ -2813,10 +2725,13 @@
         <v/>
       </c>
       <c r="G37" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+      <c r="H37" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>71</v>
       </c>
@@ -2834,10 +2749,13 @@
         <v>4750</v>
       </c>
       <c r="G38" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="H38" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>284</v>
       </c>
@@ -2855,10 +2773,13 @@
         <v/>
       </c>
       <c r="G39" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="H39" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>76</v>
       </c>
@@ -2876,10 +2797,13 @@
         <v>5750</v>
       </c>
       <c r="G40" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="H40" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>285</v>
       </c>
@@ -2897,10 +2821,13 @@
         <v/>
       </c>
       <c r="G41" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+      <c r="H41" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>81</v>
       </c>
@@ -2918,10 +2845,13 @@
         <v/>
       </c>
       <c r="G42" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+      <c r="H42" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>83</v>
       </c>
@@ -2939,10 +2869,13 @@
         <v/>
       </c>
       <c r="G43" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+      <c r="H43" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>85</v>
       </c>
@@ -2960,10 +2893,13 @@
         <v>3230</v>
       </c>
       <c r="G44" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="H44" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>89</v>
       </c>
@@ -2981,10 +2917,13 @@
         <v>4750</v>
       </c>
       <c r="G45" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="H45" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>286</v>
       </c>
@@ -3002,10 +2941,13 @@
         <v>3820</v>
       </c>
       <c r="G46" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="H46" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>287</v>
       </c>
@@ -3023,10 +2965,13 @@
         <v/>
       </c>
       <c r="G47" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+      <c r="H47" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>288</v>
       </c>
@@ -3044,10 +2989,13 @@
         <v>4100</v>
       </c>
       <c r="G48" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="H48" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>92</v>
       </c>
@@ -3065,10 +3013,13 @@
         <v/>
       </c>
       <c r="G49" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>340</v>
+      </c>
+      <c r="H49" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>96</v>
       </c>
@@ -3086,10 +3037,13 @@
         <v/>
       </c>
       <c r="G50" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+      <c r="H50" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>289</v>
       </c>
@@ -3107,10 +3061,13 @@
         <v/>
       </c>
       <c r="G51" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+      <c r="H51" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>101</v>
       </c>
@@ -3128,10 +3085,13 @@
         <v>3000</v>
       </c>
       <c r="G52" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="H52" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>106</v>
       </c>
@@ -3149,10 +3109,13 @@
         <v/>
       </c>
       <c r="G53" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+        <v>343</v>
+      </c>
+      <c r="H53" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>108</v>
       </c>
@@ -3170,10 +3133,13 @@
         <v/>
       </c>
       <c r="G54" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+      <c r="H54" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>111</v>
       </c>
@@ -3191,10 +3157,13 @@
         <v/>
       </c>
       <c r="G55" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+      <c r="H55" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>113</v>
       </c>
@@ -3212,10 +3181,13 @@
         <v>3450</v>
       </c>
       <c r="G56" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="H56" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>290</v>
       </c>
@@ -3233,10 +3205,13 @@
         <v>3830</v>
       </c>
       <c r="G57" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="H57" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>115</v>
       </c>
@@ -3254,10 +3229,13 @@
         <v>3400</v>
       </c>
       <c r="G58" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="H58" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>291</v>
       </c>
@@ -3275,10 +3253,13 @@
         <v/>
       </c>
       <c r="G59" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+      <c r="H59" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>120</v>
       </c>
@@ -3296,10 +3277,13 @@
         <v/>
       </c>
       <c r="G60" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+      <c r="H60" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>122</v>
       </c>
@@ -3317,10 +3301,13 @@
         <v>4650</v>
       </c>
       <c r="G61" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="H61" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>124</v>
       </c>
@@ -3338,10 +3325,13 @@
         <v/>
       </c>
       <c r="G62" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+      <c r="H62" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>126</v>
       </c>
@@ -3359,10 +3349,13 @@
         <v>3000</v>
       </c>
       <c r="G63" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="H63" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>130</v>
       </c>
@@ -3380,10 +3373,13 @@
         <v/>
       </c>
       <c r="G64" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="H64" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>134</v>
       </c>
@@ -3401,10 +3397,13 @@
         <v/>
       </c>
       <c r="G65" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+      <c r="H65" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>292</v>
       </c>
@@ -3422,10 +3421,13 @@
         <v>2750</v>
       </c>
       <c r="G66" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="H66" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>141</v>
       </c>
@@ -3443,10 +3445,13 @@
         <v/>
       </c>
       <c r="G67" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+      <c r="H67" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>143</v>
       </c>
@@ -3464,10 +3469,13 @@
         <v/>
       </c>
       <c r="G68" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+      <c r="H68" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>148</v>
       </c>
@@ -3485,10 +3493,13 @@
         <v/>
       </c>
       <c r="G69" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+      <c r="H69" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>151</v>
       </c>
@@ -3506,10 +3517,13 @@
         <v>3400</v>
       </c>
       <c r="G70" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="H70" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>153</v>
       </c>
@@ -3527,10 +3541,13 @@
         <v/>
       </c>
       <c r="G71" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+      <c r="H71" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>158</v>
       </c>
@@ -3548,10 +3565,13 @@
         <v/>
       </c>
       <c r="G72" s="16" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="H72" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="12" t="s">
         <v>160</v>
       </c>
@@ -3569,10 +3589,13 @@
         <v/>
       </c>
       <c r="G73" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+      <c r="H73" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
         <v>293</v>
       </c>
@@ -3590,10 +3613,13 @@
         <v>3300</v>
       </c>
       <c r="G74" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="H74" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>164</v>
       </c>
@@ -3611,10 +3637,13 @@
         <v>5550</v>
       </c>
       <c r="G75" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="H75" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>166</v>
       </c>
@@ -3632,10 +3661,13 @@
         <v/>
       </c>
       <c r="G76" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+      <c r="H76" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="12" t="s">
         <v>168</v>
       </c>
@@ -3653,10 +3685,13 @@
         <v>3700</v>
       </c>
       <c r="G77" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="H77" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>170</v>
       </c>
@@ -3674,10 +3709,13 @@
         <v>4980</v>
       </c>
       <c r="G78" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="H78" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="s">
         <v>172</v>
       </c>
@@ -3695,10 +3733,13 @@
         <v>3900</v>
       </c>
       <c r="G79" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="H79" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
         <v>294</v>
       </c>
@@ -3716,10 +3757,13 @@
         <v/>
       </c>
       <c r="G80" s="16" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+      <c r="H80" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="s">
         <v>174</v>
       </c>
@@ -3737,10 +3781,13 @@
         <v/>
       </c>
       <c r="G81" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+      <c r="H81" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>177</v>
       </c>
@@ -3758,10 +3805,13 @@
         <v/>
       </c>
       <c r="G82" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+      <c r="H82" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>179</v>
       </c>
@@ -3779,10 +3829,13 @@
         <v>3600</v>
       </c>
       <c r="G83" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H83" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>184</v>
       </c>
@@ -3800,10 +3853,13 @@
         <v>3560</v>
       </c>
       <c r="G84" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="H84" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>295</v>
       </c>
@@ -3821,10 +3877,13 @@
         <v>3000</v>
       </c>
       <c r="G85" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="H85" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>187</v>
       </c>
@@ -3842,10 +3901,13 @@
         <v>3500</v>
       </c>
       <c r="G86" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="H86" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>190</v>
       </c>
@@ -3863,10 +3925,13 @@
         <v/>
       </c>
       <c r="G87" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+      <c r="H87" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>296</v>
       </c>
@@ -3884,10 +3949,13 @@
         <v/>
       </c>
       <c r="G88" s="16" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="H88" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>194</v>
       </c>
@@ -3905,10 +3973,13 @@
         <v>2800</v>
       </c>
       <c r="G89" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="H89" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>196</v>
       </c>
@@ -3926,10 +3997,13 @@
         <v/>
       </c>
       <c r="G90" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+      <c r="H90" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>200</v>
       </c>
@@ -3947,10 +4021,13 @@
         <v/>
       </c>
       <c r="G91" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+      <c r="H91" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>202</v>
       </c>
@@ -3968,10 +4045,13 @@
         <v>2910</v>
       </c>
       <c r="G92" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="H92" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>297</v>
       </c>
@@ -3989,10 +4069,13 @@
         <v>2910</v>
       </c>
       <c r="G93" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="H93" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>207</v>
       </c>
@@ -4010,10 +4093,13 @@
         <v/>
       </c>
       <c r="G94" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+        <v>361</v>
+      </c>
+      <c r="H94" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>209</v>
       </c>
@@ -4031,10 +4117,13 @@
         <v>2650</v>
       </c>
       <c r="G95" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+      <c r="H95" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>212</v>
       </c>
@@ -4052,10 +4141,13 @@
         <v/>
       </c>
       <c r="G96" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+      <c r="H96" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>214</v>
       </c>
@@ -4073,10 +4165,13 @@
         <v>3100</v>
       </c>
       <c r="G97" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="H97" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>216</v>
       </c>
@@ -4094,10 +4189,13 @@
         <v>3200</v>
       </c>
       <c r="G98" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="H98" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>219</v>
       </c>
@@ -4115,10 +4213,13 @@
         <v/>
       </c>
       <c r="G99" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+      <c r="H99" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>298</v>
       </c>
@@ -4136,10 +4237,13 @@
         <v/>
       </c>
       <c r="G100" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="H100" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>222</v>
       </c>
@@ -4157,10 +4261,13 @@
         <v>3350</v>
       </c>
       <c r="G101" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="H101" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>225</v>
       </c>
@@ -4178,10 +4285,13 @@
         <v/>
       </c>
       <c r="G102" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+      <c r="H102" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>138</v>
       </c>
@@ -4199,10 +4309,13 @@
         <v>3100</v>
       </c>
       <c r="G103" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="H103" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>299</v>
       </c>
@@ -4220,10 +4333,13 @@
         <v>3010</v>
       </c>
       <c r="G104" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="H104" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>300</v>
       </c>
@@ -4241,10 +4357,13 @@
         <v/>
       </c>
       <c r="G105" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+      <c r="H105" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>231</v>
       </c>
@@ -4262,10 +4381,13 @@
         <v/>
       </c>
       <c r="G106" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="H106" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>233</v>
       </c>
@@ -4283,10 +4405,13 @@
         <v/>
       </c>
       <c r="G107" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+      <c r="H107" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>235</v>
       </c>
@@ -4294,7 +4419,7 @@
         <v>2620</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>431</v>
+        <v>302</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>158</v>
@@ -4304,10 +4429,13 @@
         <v>3440</v>
       </c>
       <c r="G108" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="H108" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>237</v>
       </c>
@@ -4325,10 +4453,13 @@
         <v>3410</v>
       </c>
       <c r="G109" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="H109" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
         <v>301</v>
       </c>
@@ -4346,10 +4477,13 @@
         <v/>
       </c>
       <c r="G110" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+      <c r="H110" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D111" s="2" t="s">
         <v>162</v>
       </c>
@@ -4361,10 +4495,13 @@
         <v/>
       </c>
       <c r="G111" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="H111" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D112" s="2" t="s">
         <v>163</v>
       </c>
@@ -4376,10 +4513,13 @@
         <v>3100</v>
       </c>
       <c r="G112" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="113" spans="4:7" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="H112" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="113" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D113" s="2" t="s">
         <v>165</v>
       </c>
@@ -4391,10 +4531,13 @@
         <v>4720</v>
       </c>
       <c r="G113" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="114" spans="4:7" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="H113" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="114" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D114" s="2" t="s">
         <v>167</v>
       </c>
@@ -4406,10 +4549,13 @@
         <v>3900</v>
       </c>
       <c r="G114" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="115" spans="4:7" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="H114" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="115" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D115" s="2" t="s">
         <v>169</v>
       </c>
@@ -4421,10 +4567,13 @@
         <v>4250</v>
       </c>
       <c r="G115" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="116" spans="4:7" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="H115" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="116" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D116" s="2" t="s">
         <v>171</v>
       </c>
@@ -4436,10 +4585,13 @@
         <v>3200</v>
       </c>
       <c r="G116" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="117" spans="4:7" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="H116" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="117" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D117" s="2" t="s">
         <v>173</v>
       </c>
@@ -4451,10 +4603,13 @@
         <v>4650</v>
       </c>
       <c r="G117" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="118" spans="4:7" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="H117" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="118" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D118" s="2" t="s">
         <v>175</v>
       </c>
@@ -4466,10 +4621,13 @@
         <v/>
       </c>
       <c r="G118" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="119" spans="4:7" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+      <c r="H118" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="119" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D119" s="2" t="s">
         <v>176</v>
       </c>
@@ -4481,10 +4639,13 @@
         <v>4000</v>
       </c>
       <c r="G119" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="120" spans="4:7" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="H119" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="120" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D120" s="2" t="s">
         <v>178</v>
       </c>
@@ -4496,10 +4657,13 @@
         <v>2800</v>
       </c>
       <c r="G120" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="121" spans="4:7" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="H120" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="121" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D121" s="2" t="s">
         <v>180</v>
       </c>
@@ -4511,10 +4675,13 @@
         <v/>
       </c>
       <c r="G121" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="122" spans="4:7" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+      <c r="H121" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="122" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D122" s="2" t="s">
         <v>181</v>
       </c>
@@ -4526,10 +4693,13 @@
         <v/>
       </c>
       <c r="G122" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="123" spans="4:7" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+      <c r="H122" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="123" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D123" s="2" t="s">
         <v>182</v>
       </c>
@@ -4541,10 +4711,13 @@
         <v/>
       </c>
       <c r="G123" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="124" spans="4:7" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+      <c r="H123" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="124" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D124" s="2" t="s">
         <v>183</v>
       </c>
@@ -4556,10 +4729,13 @@
         <v>3650</v>
       </c>
       <c r="G124" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="125" spans="4:7" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="H124" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="125" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D125" s="2" t="s">
         <v>185</v>
       </c>
@@ -4571,10 +4747,13 @@
         <v/>
       </c>
       <c r="G125" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="126" spans="4:7" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+      <c r="H125" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="126" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D126" s="2" t="s">
         <v>186</v>
       </c>
@@ -4586,10 +4765,13 @@
         <v>2680</v>
       </c>
       <c r="G126" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="127" spans="4:7" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+      <c r="H126" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="127" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D127" s="2" t="s">
         <v>188</v>
       </c>
@@ -4601,10 +4783,13 @@
         <v/>
       </c>
       <c r="G127" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="128" spans="4:7" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+      <c r="H127" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="128" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D128" s="2" t="s">
         <v>189</v>
       </c>
@@ -4616,10 +4801,13 @@
         <v>2850</v>
       </c>
       <c r="G128" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="129" spans="4:7" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+      <c r="H128" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="129" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D129" s="2" t="s">
         <v>191</v>
       </c>
@@ -4631,10 +4819,13 @@
         <v/>
       </c>
       <c r="G129" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="130" spans="4:7" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+      <c r="H129" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="130" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D130" s="2" t="s">
         <v>192</v>
       </c>
@@ -4646,10 +4837,13 @@
         <v/>
       </c>
       <c r="G130" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="131" spans="4:7" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="H130" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="131" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D131" s="2" t="s">
         <v>193</v>
       </c>
@@ -4661,10 +4855,13 @@
         <v>5040</v>
       </c>
       <c r="G131" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="132" spans="4:7" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+      <c r="H131" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="132" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D132" s="2" t="s">
         <v>195</v>
       </c>
@@ -4676,10 +4873,13 @@
         <v>2900</v>
       </c>
       <c r="G132" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="133" spans="4:7" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+      <c r="H132" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="133" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D133" s="2" t="s">
         <v>197</v>
       </c>
@@ -4691,10 +4891,13 @@
         <v/>
       </c>
       <c r="G133" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="134" spans="4:7" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+      <c r="H133" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="134" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D134" s="2" t="s">
         <v>198</v>
       </c>
@@ -4706,10 +4909,13 @@
         <v/>
       </c>
       <c r="G134" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="135" spans="4:7" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="H134" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="135" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D135" s="2" t="s">
         <v>199</v>
       </c>
@@ -4721,10 +4927,13 @@
         <v>2950</v>
       </c>
       <c r="G135" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="136" spans="4:7" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="H135" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="136" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D136" s="2" t="s">
         <v>201</v>
       </c>
@@ -4736,10 +4945,13 @@
         <v>4350</v>
       </c>
       <c r="G136" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="137" spans="4:7" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+      <c r="H136" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="137" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D137" s="2" t="s">
         <v>203</v>
       </c>
@@ -4751,10 +4963,13 @@
         <v/>
       </c>
       <c r="G137" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="138" spans="4:7" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="H137" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="138" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D138" s="2" t="s">
         <v>204</v>
       </c>
@@ -4766,10 +4981,13 @@
         <v/>
       </c>
       <c r="G138" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="139" spans="4:7" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="H138" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="139" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D139" s="2" t="s">
         <v>205</v>
       </c>
@@ -4781,10 +4999,13 @@
         <v/>
       </c>
       <c r="G139" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="140" spans="4:7" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+      <c r="H139" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="140" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D140" s="2" t="s">
         <v>206</v>
       </c>
@@ -4796,10 +5017,13 @@
         <v>3150</v>
       </c>
       <c r="G140" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="141" spans="4:7" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+      <c r="H140" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="141" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D141" s="2" t="s">
         <v>208</v>
       </c>
@@ -4811,10 +5035,13 @@
         <v>5720</v>
       </c>
       <c r="G141" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="142" spans="4:7" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+      <c r="H141" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="142" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D142" s="2" t="s">
         <v>210</v>
       </c>
@@ -4826,10 +5053,13 @@
         <v/>
       </c>
       <c r="G142" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="143" spans="4:7" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+      <c r="H142" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="143" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D143" s="2" t="s">
         <v>211</v>
       </c>
@@ -4841,10 +5071,13 @@
         <v>4150</v>
       </c>
       <c r="G143" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="144" spans="4:7" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="H143" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="144" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D144" s="2" t="s">
         <v>213</v>
       </c>
@@ -4856,10 +5089,13 @@
         <v>3150</v>
       </c>
       <c r="G144" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="145" spans="4:7" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="H144" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="145" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D145" s="2" t="s">
         <v>215</v>
       </c>
@@ -4871,10 +5107,13 @@
         <v>3600</v>
       </c>
       <c r="G145" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="146" spans="4:7" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="H145" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="146" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D146" s="2" t="s">
         <v>217</v>
       </c>
@@ -4886,10 +5125,13 @@
         <v/>
       </c>
       <c r="G146" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="147" spans="4:7" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+      <c r="H146" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="147" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D147" s="2" t="s">
         <v>218</v>
       </c>
@@ -4901,10 +5143,13 @@
         <v>3120</v>
       </c>
       <c r="G147" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="148" spans="4:7" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+      <c r="H147" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="148" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D148" s="2" t="s">
         <v>220</v>
       </c>
@@ -4916,10 +5161,13 @@
         <v/>
       </c>
       <c r="G148" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="149" spans="4:7" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+      <c r="H148" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="149" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D149" s="2" t="s">
         <v>221</v>
       </c>
@@ -4931,10 +5179,13 @@
         <v>2925</v>
       </c>
       <c r="G149" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="150" spans="4:7" x14ac:dyDescent="0.2">
+        <v>386</v>
+      </c>
+      <c r="H149" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="150" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D150" s="2" t="s">
         <v>223</v>
       </c>
@@ -4946,10 +5197,13 @@
         <v/>
       </c>
       <c r="G150" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="151" spans="4:7" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+      <c r="H150" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="151" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D151" s="2" t="s">
         <v>224</v>
       </c>
@@ -4961,10 +5215,13 @@
         <v>3600</v>
       </c>
       <c r="G151" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="152" spans="4:7" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+      <c r="H151" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="152" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D152" s="2" t="s">
         <v>226</v>
       </c>
@@ -4976,10 +5233,13 @@
         <v>2650</v>
       </c>
       <c r="G152" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="153" spans="4:7" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="H152" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="153" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D153" s="2" t="s">
         <v>227</v>
       </c>
@@ -4991,10 +5251,13 @@
         <v/>
       </c>
       <c r="G153" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="154" spans="4:7" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+      <c r="H153" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="154" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D154" s="2" t="s">
         <v>228</v>
       </c>
@@ -5006,10 +5269,13 @@
         <v/>
       </c>
       <c r="G154" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="155" spans="4:7" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+      <c r="H154" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="155" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D155" s="2" t="s">
         <v>229</v>
       </c>
@@ -5021,10 +5287,13 @@
         <v/>
       </c>
       <c r="G155" s="16" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="156" spans="4:7" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+      <c r="H155" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="156" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D156" s="2" t="s">
         <v>157</v>
       </c>
@@ -5036,10 +5305,13 @@
         <v/>
       </c>
       <c r="G156" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="157" spans="4:7" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+      <c r="H156" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="157" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D157" s="2" t="s">
         <v>230</v>
       </c>
@@ -5051,10 +5323,13 @@
         <v>2950</v>
       </c>
       <c r="G157" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="158" spans="4:7" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+      <c r="H157" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="158" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D158" s="2" t="s">
         <v>232</v>
       </c>
@@ -5066,10 +5341,13 @@
         <v>4180</v>
       </c>
       <c r="G158" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="159" spans="4:7" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+      <c r="H158" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="159" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D159" s="2" t="s">
         <v>234</v>
       </c>
@@ -5081,10 +5359,13 @@
         <v>2620</v>
       </c>
       <c r="G159" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="160" spans="4:7" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="H159" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="160" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D160" s="2" t="s">
         <v>236</v>
       </c>
@@ -5096,10 +5377,13 @@
         <v>4400</v>
       </c>
       <c r="G160" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+      <c r="H160" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="161" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D161" s="2" t="s">
         <v>238</v>
       </c>
@@ -5111,17 +5395,13 @@
         <v/>
       </c>
       <c r="G161" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C162" s="18"/>
-      <c r="D162" s="18"/>
-      <c r="E162" s="18"/>
-      <c r="F162" s="18"/>
-      <c r="G162" s="18"/>
-    </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+      <c r="H161" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="163" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D163" s="2" t="s">
         <v>239</v>
       </c>
@@ -5130,10 +5410,13 @@
         <v/>
       </c>
       <c r="G163" s="17" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+      <c r="H163" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="164" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D164" s="2" t="s">
         <v>240</v>
       </c>
@@ -5142,10 +5425,13 @@
         <v/>
       </c>
       <c r="G164" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+      <c r="H164" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="165" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D165" s="2" t="s">
         <v>241</v>
       </c>
@@ -5154,10 +5440,13 @@
         <v/>
       </c>
       <c r="G165" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+      <c r="H165" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="166" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D166" s="2" t="s">
         <v>242</v>
       </c>
@@ -5166,10 +5455,13 @@
         <v/>
       </c>
       <c r="G166" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+      <c r="H166" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="167" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D167" s="2" t="s">
         <v>243</v>
       </c>
@@ -5178,10 +5470,13 @@
         <v/>
       </c>
       <c r="G167" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+      <c r="H167" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="168" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D168" s="2" t="s">
         <v>244</v>
       </c>
@@ -5190,10 +5485,13 @@
         <v/>
       </c>
       <c r="G168" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+      <c r="H168" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="169" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D169" s="2" t="s">
         <v>245</v>
       </c>
@@ -5202,10 +5500,13 @@
         <v/>
       </c>
       <c r="G169" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="H169" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="170" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D170" s="2" t="s">
         <v>246</v>
       </c>
@@ -5214,10 +5515,13 @@
         <v/>
       </c>
       <c r="G170" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+      <c r="H170" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="171" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D171" s="2" t="s">
         <v>247</v>
       </c>
@@ -5226,10 +5530,13 @@
         <v/>
       </c>
       <c r="G171" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+      <c r="H171" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="172" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D172" s="2" t="s">
         <v>248</v>
       </c>
@@ -5238,10 +5545,13 @@
         <v/>
       </c>
       <c r="G172" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+      <c r="H172" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="173" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D173" s="2" t="s">
         <v>249</v>
       </c>
@@ -5250,10 +5560,13 @@
         <v/>
       </c>
       <c r="G173" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+      <c r="H173" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="174" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D174" s="2" t="s">
         <v>250</v>
       </c>
@@ -5262,10 +5575,13 @@
         <v/>
       </c>
       <c r="G174" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="H174" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="175" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D175" s="2" t="s">
         <v>251</v>
       </c>
@@ -5274,10 +5590,13 @@
         <v/>
       </c>
       <c r="G175" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+      <c r="H175" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="176" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D176" s="2" t="s">
         <v>252</v>
       </c>
@@ -5286,10 +5605,13 @@
         <v/>
       </c>
       <c r="G176" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="177" spans="4:7" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+      <c r="H176" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="177" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D177" s="2" t="s">
         <v>253</v>
       </c>
@@ -5298,10 +5620,13 @@
         <v/>
       </c>
       <c r="G177" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="178" spans="4:7" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+      <c r="H177" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="178" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D178" s="2" t="s">
         <v>254</v>
       </c>
@@ -5310,10 +5635,13 @@
         <v/>
       </c>
       <c r="G178" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="179" spans="4:7" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+      <c r="H178" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="179" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D179" s="2" t="s">
         <v>255</v>
       </c>
@@ -5324,8 +5652,11 @@
       <c r="G179" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="180" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="H179" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="180" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D180" s="2" t="s">
         <v>256</v>
       </c>
@@ -5334,10 +5665,13 @@
         <v/>
       </c>
       <c r="G180" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="181" spans="4:7" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+      <c r="H180" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="181" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D181" s="2" t="s">
         <v>257</v>
       </c>
@@ -5346,10 +5680,13 @@
         <v/>
       </c>
       <c r="G181" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="182" spans="4:7" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+      <c r="H181" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="182" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D182" s="2" t="s">
         <v>258</v>
       </c>
@@ -5358,10 +5695,13 @@
         <v/>
       </c>
       <c r="G182" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="183" spans="4:7" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+      <c r="H182" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="183" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D183" s="2" t="s">
         <v>259</v>
       </c>
@@ -5370,10 +5710,13 @@
         <v/>
       </c>
       <c r="G183" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="184" spans="4:7" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+      <c r="H183" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="184" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D184" s="2" t="s">
         <v>260</v>
       </c>
@@ -5382,10 +5725,13 @@
         <v/>
       </c>
       <c r="G184" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="185" spans="4:7" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+      <c r="H184" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="185" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D185" s="2" t="s">
         <v>261</v>
       </c>
@@ -5394,10 +5740,13 @@
         <v/>
       </c>
       <c r="G185" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="186" spans="4:7" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+      <c r="H185" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="186" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D186" s="2" t="s">
         <v>262</v>
       </c>
@@ -5406,10 +5755,13 @@
         <v/>
       </c>
       <c r="G186" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="187" spans="4:7" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="H186" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="187" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D187" s="2" t="s">
         <v>263</v>
       </c>
@@ -5418,10 +5770,13 @@
         <v/>
       </c>
       <c r="G187" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="188" spans="4:7" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+      <c r="H187" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="188" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D188" s="2" t="s">
         <v>264</v>
       </c>
@@ -5430,10 +5785,13 @@
         <v/>
       </c>
       <c r="G188" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="189" spans="4:7" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="H188" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="189" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D189" s="2" t="s">
         <v>265</v>
       </c>
@@ -5442,7 +5800,10 @@
         <v/>
       </c>
       <c r="G189" t="s">
-        <v>460</v>
+        <v>418</v>
+      </c>
+      <c r="H189" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>